<commit_message>
updated holiday extra pay
</commit_message>
<xml_diff>
--- a/processed_files/INVOICE - 2023-11-16 - 2023-11-30.xlsx
+++ b/processed_files/INVOICE - 2023-11-16 - 2023-11-30.xlsx
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="C8" s="26" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="26" t="n">
         <v>2023</v>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="C40" s="61" t="inlineStr">
         <is>
-          <t>12.06.23</t>
+          <t>12.07.23</t>
         </is>
       </c>
       <c r="D40" s="58" t="n"/>
@@ -10859,10 +10859,10 @@
         <v>45253.29097222222</v>
       </c>
       <c r="S118" t="n">
-        <v>0</v>
+        <v>419</v>
       </c>
       <c r="T118" t="n">
-        <v>0</v>
+        <v>6.98</v>
       </c>
     </row>
     <row r="119">
@@ -10938,10 +10938,10 @@
         <v>45253.30069444444</v>
       </c>
       <c r="S119" t="n">
-        <v>13</v>
+        <v>433</v>
       </c>
       <c r="T119" t="n">
-        <v>0.22</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="120">
@@ -11017,10 +11017,10 @@
         <v>45253.62291666667</v>
       </c>
       <c r="S120" t="n">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="T120" t="n">
-        <v>7.95</v>
+        <v>8.130000000000001</v>
       </c>
     </row>
     <row r="121">
@@ -11096,10 +11096,10 @@
         <v>45253.625</v>
       </c>
       <c r="S121" t="n">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="T121" t="n">
-        <v>8</v>
+        <v>8.08</v>
       </c>
     </row>
     <row r="122">
@@ -11552,10 +11552,10 @@
         <v>45253.96180555555</v>
       </c>
       <c r="S127" t="n">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="T127" t="n">
-        <v>8.15</v>
+        <v>8.23</v>
       </c>
     </row>
     <row r="128">
@@ -11631,10 +11631,10 @@
         <v>45253.96180555555</v>
       </c>
       <c r="S128" t="n">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="T128" t="n">
-        <v>8.02</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="129">
@@ -11710,10 +11710,10 @@
         <v>45253.96527777778</v>
       </c>
       <c r="S129" t="n">
-        <v>480</v>
+        <v>490</v>
       </c>
       <c r="T129" t="n">
-        <v>8</v>
+        <v>8.17</v>
       </c>
     </row>
     <row r="130">
@@ -11789,10 +11789,10 @@
         <v>45254</v>
       </c>
       <c r="S130" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="T130" t="n">
-        <v>0</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="131">
@@ -11868,10 +11868,10 @@
         <v>45254</v>
       </c>
       <c r="S131" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="T131" t="n">
-        <v>0</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="132">

</xml_diff>